<commit_message>
Includes median in position analysis and improves visualization
</commit_message>
<xml_diff>
--- a/DataCollection/Correlation/Rank_Correlation_Player_Stats_Playoffs.xlsx
+++ b/DataCollection/Correlation/Rank_Correlation_Player_Stats_Playoffs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
@@ -52,74 +52,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -393,10 +325,10 @@
   <dimension ref="A1:V139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2459,7 +2391,7 @@
         <v>0.3647058823529412</v>
       </c>
       <c r="N29" t="n">
-        <v>0.2588235294117647</v>
+        <v>0.2382352941176471</v>
       </c>
       <c r="O29" t="n">
         <v>0.4294117647058824</v>

</xml_diff>